<commit_message>
cleaned up issues with spreadsheets
</commit_message>
<xml_diff>
--- a/01_spreadsheet/results/bold_jul252019.xlsx
+++ b/01_spreadsheet/results/bold_jul252019.xlsx
@@ -1,244 +1,354 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jasmine/tmp/bold-workflow/01_spreadsheet/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
-    <sheet name="Voucher Info" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Taxonomy" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Specimen Details" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Collection Data" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Voucher Info" sheetId="1" r:id="rId1"/>
+    <sheet name="Taxonomy" sheetId="2" r:id="rId2"/>
+    <sheet name="Specimen Details" sheetId="3" r:id="rId3"/>
+    <sheet name="Collection Data" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
-  <si>
-    <t xml:space="preserve">Sample ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Field ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Museum ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collection Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Institution Storing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTM1849</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">University of British Columbia, Herbarium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTM1850</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTM1854</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTM1855</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTM1856</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phylum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subfamily</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identifier Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identifier Institution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identification Method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxonomy Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sam Starko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">University of British Columbia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soren Huber, Patrick T. Martone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reproduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Life Stage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extra Info</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voucher Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tissue Descriptor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Associated Taxa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Associated Specimens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">External URLs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collectors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collection Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country/Ocean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State/Province</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exact Site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Longitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elevation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elevation Precision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth Precision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPS Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordinate Accuracy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collection Date Accuracy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Habitat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sampling Protocol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collection Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Site Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collection Event ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05-Jun-2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">British Columbia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hakai</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="104">
+  <si>
+    <t>Sample ID</t>
+  </si>
+  <si>
+    <t>Field ID</t>
+  </si>
+  <si>
+    <t>Museum ID</t>
+  </si>
+  <si>
+    <t>Collection Code</t>
+  </si>
+  <si>
+    <t>Institution Storing</t>
+  </si>
+  <si>
+    <t>PTM1849</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>University of British Columbia, Herbarium</t>
+  </si>
+  <si>
+    <t>PTM1850</t>
+  </si>
+  <si>
+    <t>PTM1854</t>
+  </si>
+  <si>
+    <t>PTM1855</t>
+  </si>
+  <si>
+    <t>PTM1856</t>
+  </si>
+  <si>
+    <t>LML025</t>
+  </si>
+  <si>
+    <t>pinnacle offshore from Island</t>
+  </si>
+  <si>
+    <t>SRH13</t>
+  </si>
+  <si>
+    <t>SRH14</t>
+  </si>
+  <si>
+    <t>SRH33</t>
+  </si>
+  <si>
+    <t>SRH37</t>
+  </si>
+  <si>
+    <t>SRH40</t>
+  </si>
+  <si>
+    <t>SRH49</t>
+  </si>
+  <si>
+    <t>Phylum</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Subfamily</t>
+  </si>
+  <si>
+    <t>Genus</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>Identifier Email</t>
+  </si>
+  <si>
+    <t>Identifier Institution</t>
+  </si>
+  <si>
+    <t>Identification Method</t>
+  </si>
+  <si>
+    <t>Taxonomy Notes</t>
+  </si>
+  <si>
+    <t>Rhodophyta</t>
+  </si>
+  <si>
+    <t>Florideophyceae</t>
+  </si>
+  <si>
+    <t>Corallinales</t>
+  </si>
+  <si>
+    <t>Corallinaceae</t>
+  </si>
+  <si>
+    <t>Corallinoideae</t>
+  </si>
+  <si>
+    <t>Bossiella</t>
+  </si>
+  <si>
+    <t>Bossiella frondifera</t>
+  </si>
+  <si>
+    <t>Sam Starko</t>
+  </si>
+  <si>
+    <t>University of British Columbia</t>
+  </si>
+  <si>
+    <t>Bossiella plumosa</t>
+  </si>
+  <si>
+    <t>Corallina Sp. 1 california?</t>
+  </si>
+  <si>
+    <t>Soren Huber, Patrick T. Martone</t>
+  </si>
+  <si>
+    <t>Bossiella hakaiensis?</t>
+  </si>
+  <si>
+    <t>Bossiella manzae? (reptans?)</t>
+  </si>
+  <si>
+    <t>Coralline</t>
+  </si>
+  <si>
+    <t>Coralline crust</t>
+  </si>
+  <si>
+    <t>Corallina</t>
+  </si>
+  <si>
+    <t>Corallina vancouveriensis</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Reproduction</t>
+  </si>
+  <si>
+    <t>Life Stage</t>
+  </si>
+  <si>
+    <t>Extra Info</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Voucher Status</t>
+  </si>
+  <si>
+    <t>Tissue Descriptor</t>
+  </si>
+  <si>
+    <t>Associated Taxa</t>
+  </si>
+  <si>
+    <t>Associated Specimens</t>
+  </si>
+  <si>
+    <t>External URLs</t>
+  </si>
+  <si>
+    <t>Collectors</t>
+  </si>
+  <si>
+    <t>Collection Date</t>
+  </si>
+  <si>
+    <t>Country/Ocean</t>
+  </si>
+  <si>
+    <t>State/Province</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>Exact Site</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Elevation</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Elevation Precision</t>
+  </si>
+  <si>
+    <t>Depth Precision</t>
+  </si>
+  <si>
+    <t>GPS Source</t>
+  </si>
+  <si>
+    <t>Coordinate Accuracy</t>
+  </si>
+  <si>
+    <t>Event Time</t>
+  </si>
+  <si>
+    <t>Collection Date Accuracy</t>
+  </si>
+  <si>
+    <t>Habitat</t>
+  </si>
+  <si>
+    <t>Sampling Protocol</t>
+  </si>
+  <si>
+    <t>Collection Notes</t>
+  </si>
+  <si>
+    <t>Site Code</t>
+  </si>
+  <si>
+    <t>Collection Event ID</t>
+  </si>
+  <si>
+    <t>05-Jun-2019</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>British Columbia</t>
+  </si>
+  <si>
+    <t>Hakai</t>
   </si>
   <si>
     <t xml:space="preserve"> North Beach Bench</t>
   </si>
   <si>
-    <t xml:space="preserve">Coralline X - Plot 3 exclusion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06-Jun-2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04-Jun-2019</t>
+    <t>Coralline X - Plot 3 exclusion</t>
+  </si>
+  <si>
+    <t>06-Jun-2019</t>
+  </si>
+  <si>
+    <t>04-Jun-2019</t>
   </si>
   <si>
     <t xml:space="preserve"> Fifth Beach</t>
   </si>
   <si>
-    <t xml:space="preserve">Difficult to determine.  Large compared to other Sp. 1 CA in viciniy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coralline X-Plot 5C, not sure if hakaiensis or reptans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06-June-2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coralline X-Plot 2C, not sure if manzae or reptans</t>
+    <t>Difficult to determine.  Large compared to other Sp. 1 CA in viciniy.</t>
+  </si>
+  <si>
+    <t>Coralline X-Plot 5C, not sure if hakaiensis or reptans</t>
+  </si>
+  <si>
+    <t>06-June-2019</t>
+  </si>
+  <si>
+    <t>Coralline X-Plot 2C, not sure if manzae or reptans</t>
+  </si>
+  <si>
+    <t>12-May-2019</t>
+  </si>
+  <si>
+    <t>North Bowyer Island</t>
+  </si>
+  <si>
+    <t>49.431987</t>
+  </si>
+  <si>
+    <t>-123.274532</t>
+  </si>
+  <si>
+    <t>14-June-2018</t>
+  </si>
+  <si>
+    <t>North Beach</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hakai</t>
+  </si>
+  <si>
+    <t>16-June-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Howe Sound</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -274,6 +384,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -555,14 +671,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -579,14 +697,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2"/>
       <c r="D2" t="s">
         <v>6</v>
       </c>
@@ -594,14 +711,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3"/>
       <c r="D3" t="s">
         <v>6</v>
       </c>
@@ -609,14 +725,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4"/>
       <c r="D4" t="s">
         <v>6</v>
       </c>
@@ -624,14 +739,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5"/>
       <c r="D5" t="s">
         <v>6</v>
       </c>
@@ -639,14 +753,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6"/>
       <c r="D6" t="s">
         <v>6</v>
       </c>
@@ -654,80 +767,197 @@
         <v>7</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="21" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="K1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="L1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
         <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="L2" t="s">
         <v>6</v>
@@ -736,25 +966,39 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
+        <v>41</v>
+      </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="L3" t="s">
         <v>6</v>
@@ -763,25 +1007,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="J4" t="s">
         <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="L4" t="s">
         <v>6</v>
@@ -790,25 +1030,39 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="J5" t="s">
         <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="L5" t="s">
         <v>6</v>
@@ -817,87 +1071,366 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="J6" t="s">
         <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="L6" t="s">
         <v>6</v>
       </c>
       <c r="M6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M13" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="K1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2"/>
       <c r="C2" t="s">
         <v>6</v>
       </c>
@@ -926,11 +1459,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3"/>
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -959,11 +1491,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4"/>
       <c r="C4" t="s">
         <v>6</v>
       </c>
@@ -992,11 +1523,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5"/>
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -1025,11 +1555,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6"/>
       <c r="C6" t="s">
         <v>6</v>
       </c>
@@ -1055,95 +1584,325 @@
         <v>6</v>
       </c>
       <c r="K6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="K1" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="M1" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="N1" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="O1" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="P1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="Q1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="R1" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="S1" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="T1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="U1" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="V1" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="W1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1151,25 +1910,23 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2"/>
-      <c r="J2"/>
+        <v>86</v>
+      </c>
       <c r="K2" t="s">
         <v>6</v>
       </c>
@@ -1194,19 +1951,17 @@
       <c r="R2" t="s">
         <v>6</v>
       </c>
-      <c r="S2"/>
       <c r="T2" t="s">
         <v>6</v>
       </c>
-      <c r="U2"/>
       <c r="V2" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="W2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1214,25 +1969,23 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3"/>
-      <c r="J3"/>
+        <v>86</v>
+      </c>
       <c r="K3" t="s">
         <v>6</v>
       </c>
@@ -1257,19 +2010,17 @@
       <c r="R3" t="s">
         <v>6</v>
       </c>
-      <c r="S3"/>
       <c r="T3" t="s">
         <v>6</v>
       </c>
-      <c r="U3"/>
       <c r="V3" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="W3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1277,25 +2028,23 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I4"/>
-      <c r="J4"/>
+        <v>90</v>
+      </c>
       <c r="K4" t="s">
         <v>6</v>
       </c>
@@ -1320,19 +2069,17 @@
       <c r="R4" t="s">
         <v>6</v>
       </c>
-      <c r="S4"/>
       <c r="T4" t="s">
         <v>6</v>
       </c>
-      <c r="U4"/>
       <c r="V4" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="W4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1340,25 +2087,23 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5"/>
-      <c r="J5"/>
+        <v>86</v>
+      </c>
       <c r="K5" t="s">
         <v>6</v>
       </c>
@@ -1383,19 +2128,17 @@
       <c r="R5" t="s">
         <v>6</v>
       </c>
-      <c r="S5"/>
       <c r="T5" t="s">
         <v>6</v>
       </c>
-      <c r="U5"/>
       <c r="V5" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="W5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1403,25 +2146,23 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6"/>
-      <c r="J6"/>
+        <v>86</v>
+      </c>
       <c r="K6" t="s">
         <v>6</v>
       </c>
@@ -1446,20 +2187,398 @@
       <c r="R6" t="s">
         <v>6</v>
       </c>
-      <c r="S6"/>
       <c r="T6" t="s">
         <v>6</v>
       </c>
-      <c r="U6"/>
       <c r="V6" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="W6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J7" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" t="s">
+        <v>6</v>
+      </c>
+      <c r="T7" t="s">
+        <v>6</v>
+      </c>
+      <c r="U7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" t="s">
+        <v>100</v>
+      </c>
+      <c r="K8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>6</v>
+      </c>
+      <c r="R8" t="s">
+        <v>6</v>
+      </c>
+      <c r="T8" t="s">
+        <v>6</v>
+      </c>
+      <c r="W8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" t="s">
+        <v>100</v>
+      </c>
+      <c r="K9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" t="s">
+        <v>6</v>
+      </c>
+      <c r="T9" t="s">
+        <v>6</v>
+      </c>
+      <c r="W9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" t="s">
+        <v>100</v>
+      </c>
+      <c r="K10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N10" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" t="s">
+        <v>6</v>
+      </c>
+      <c r="T10" t="s">
+        <v>6</v>
+      </c>
+      <c r="W10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H11" t="s">
+        <v>100</v>
+      </c>
+      <c r="K11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" t="s">
+        <v>6</v>
+      </c>
+      <c r="N11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" t="s">
+        <v>6</v>
+      </c>
+      <c r="T11" t="s">
+        <v>6</v>
+      </c>
+      <c r="W11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" t="s">
+        <v>100</v>
+      </c>
+      <c r="K12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R12" t="s">
+        <v>6</v>
+      </c>
+      <c r="T12" t="s">
+        <v>6</v>
+      </c>
+      <c r="W12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" t="s">
+        <v>100</v>
+      </c>
+      <c r="K13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13" t="s">
+        <v>6</v>
+      </c>
+      <c r="T13" t="s">
+        <v>6</v>
+      </c>
+      <c r="W13" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates to the spreadsheet
</commit_message>
<xml_diff>
--- a/01_spreadsheet/results/bold_jul252019.xlsx
+++ b/01_spreadsheet/results/bold_jul252019.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="1720" yWindow="460" windowWidth="27760" windowHeight="17540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Voucher Info" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="105">
   <si>
     <t>Sample ID</t>
   </si>
@@ -302,9 +302,6 @@
     <t>04-Jun-2019</t>
   </si>
   <si>
-    <t xml:space="preserve"> Fifth Beach</t>
-  </si>
-  <si>
     <t>Difficult to determine.  Large compared to other Sp. 1 CA in viciniy.</t>
   </si>
   <si>
@@ -341,7 +338,13 @@
     <t>16-June-2018</t>
   </si>
   <si>
-    <t xml:space="preserve"> Howe Sound</t>
+    <t>North Beach Bench</t>
+  </si>
+  <si>
+    <t>Fifth Beach</t>
+  </si>
+  <si>
+    <t>Howe Sound</t>
   </si>
 </sst>
 </file>
@@ -674,7 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -1821,8 +1824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2043,37 +2046,37 @@
         <v>85</v>
       </c>
       <c r="H4" t="s">
+        <v>103</v>
+      </c>
+      <c r="K4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>6</v>
+      </c>
+      <c r="R4" t="s">
+        <v>6</v>
+      </c>
+      <c r="T4" t="s">
+        <v>6</v>
+      </c>
+      <c r="V4" t="s">
         <v>90</v>
-      </c>
-      <c r="K4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N4" t="s">
-        <v>6</v>
-      </c>
-      <c r="O4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P4" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>6</v>
-      </c>
-      <c r="R4" t="s">
-        <v>6</v>
-      </c>
-      <c r="T4" t="s">
-        <v>6</v>
-      </c>
-      <c r="V4" t="s">
-        <v>91</v>
       </c>
       <c r="W4" t="s">
         <v>6</v>
@@ -2102,7 +2105,7 @@
         <v>85</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="K5" t="s">
         <v>6</v>
@@ -2132,7 +2135,7 @@
         <v>6</v>
       </c>
       <c r="V5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="W5" t="s">
         <v>6</v>
@@ -2146,7 +2149,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
         <v>83</v>
@@ -2161,7 +2164,7 @@
         <v>85</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="K6" t="s">
         <v>6</v>
@@ -2191,7 +2194,7 @@
         <v>6</v>
       </c>
       <c r="V6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W6" t="s">
         <v>6</v>
@@ -2205,7 +2208,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
         <v>83</v>
@@ -2217,16 +2220,16 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I7" t="s">
         <v>96</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>97</v>
-      </c>
-      <c r="J7" t="s">
-        <v>98</v>
       </c>
       <c r="K7" t="s">
         <v>6</v>
@@ -2267,7 +2270,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
         <v>83</v>
@@ -2279,10 +2282,10 @@
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="H8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K8" t="s">
         <v>6</v>
@@ -2320,7 +2323,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D9" t="s">
         <v>83</v>
@@ -2332,10 +2335,10 @@
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K9" t="s">
         <v>6</v>
@@ -2373,7 +2376,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" t="s">
         <v>83</v>
@@ -2385,10 +2388,10 @@
         <v>6</v>
       </c>
       <c r="G10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K10" t="s">
         <v>6</v>
@@ -2426,7 +2429,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" t="s">
         <v>83</v>
@@ -2438,10 +2441,10 @@
         <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K11" t="s">
         <v>6</v>
@@ -2479,7 +2482,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" t="s">
         <v>83</v>
@@ -2491,10 +2494,10 @@
         <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K12" t="s">
         <v>6</v>
@@ -2532,7 +2535,7 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D13" t="s">
         <v>83</v>
@@ -2544,10 +2547,10 @@
         <v>6</v>
       </c>
       <c r="G13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K13" t="s">
         <v>6</v>

</xml_diff>